<commit_message>
output discrepant roles with toh num of texts
</commit_message>
<xml_diff>
--- a/unmatched_persons_discrepant_roles.xlsx
+++ b/unmatched_persons_discrepant_roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4124AFD-69AE-7544-AB2C-6F54BDBF59FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B77764-0FA1-4B4C-9035-D89975FAF75A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16100" activeTab="1" xr2:uid="{AA1A54E2-02A9-434E-B49F-C824DE424E33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="15820" xr2:uid="{AA1A54E2-02A9-434E-B49F-C824DE424E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -843,12 +843,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -863,8 +869,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1189,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D804DCDA-38F3-6F46-A929-08C51F317D4A}">
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,23 +1747,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1920,23 +1927,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>76</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4300,23 +4307,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156">
+    <row r="156" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
         <v>62</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E156" t="s">
-        <v>8</v>
-      </c>
-      <c r="F156" t="s">
+      <c r="E156" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F156" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4592,7 +4599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526F31F5-B02A-5740-87CE-9D773BE86CC7}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>